<commit_message>
Added dates for axis among other things
</commit_message>
<xml_diff>
--- a/totalt-antal-konstaterade-covid-fall.xlsx
+++ b/totalt-antal-konstaterade-covid-fall.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\DARC_Extra\Prognostisering baserad på 1177 MÅ\Geografiindelat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\DARC_Extra\Prognostisering baserad på 1177 MÅ\R-talet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E61861-59C3-4F39-8BCF-6121801EC7BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F58A5BC-8C35-4779-997E-5F86931F4ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Underlag" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="361">
   <si>
     <t>Nya konstaterade personer</t>
   </si>
@@ -1101,6 +1101,21 @@
   </si>
   <si>
     <t>17 februari 2021</t>
+  </si>
+  <si>
+    <t>18 februari 2021</t>
+  </si>
+  <si>
+    <t>19 februari 2021</t>
+  </si>
+  <si>
+    <t>20 februari 2021</t>
+  </si>
+  <si>
+    <t>21 februari 2021</t>
+  </si>
+  <si>
+    <t>22 februari 2021</t>
   </si>
 </sst>
 </file>
@@ -1434,11 +1449,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C354"/>
+  <dimension ref="A1:C359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A353" sqref="A353:A354"/>
+      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A358" sqref="A358:A359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5292,10 +5307,10 @@
         <v>351</v>
       </c>
       <c r="B350" s="7">
-        <v>104440</v>
+        <v>104691</v>
       </c>
       <c r="C350" s="7">
-        <v>104</v>
+        <v>355</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.3">
@@ -5303,10 +5318,10 @@
         <v>352</v>
       </c>
       <c r="B351" s="1">
-        <v>104657</v>
+        <v>104913</v>
       </c>
       <c r="C351" s="1">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.3">
@@ -5314,10 +5329,10 @@
         <v>353</v>
       </c>
       <c r="B352" s="1">
-        <v>105256</v>
+        <v>105260</v>
       </c>
       <c r="C352" s="1">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.3">
@@ -5325,10 +5340,10 @@
         <v>354</v>
       </c>
       <c r="B353" s="1">
-        <v>105735</v>
+        <v>105738</v>
       </c>
       <c r="C353" s="1">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.3">
@@ -5336,10 +5351,65 @@
         <v>355</v>
       </c>
       <c r="B354" s="1">
-        <v>106352</v>
+        <v>106350</v>
       </c>
       <c r="C354" s="1">
-        <v>614</v>
+        <v>612</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A355" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="B355" s="1">
+        <v>106939</v>
+      </c>
+      <c r="C355" s="1">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A356" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B356" s="1">
+        <v>107535</v>
+      </c>
+      <c r="C356" s="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A357" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="B357" s="1">
+        <v>107859</v>
+      </c>
+      <c r="C357" s="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A358" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="B358" s="1">
+        <v>108082</v>
+      </c>
+      <c r="C358" s="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A359" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="B359" s="1">
+        <v>108352</v>
+      </c>
+      <c r="C359" s="1">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a bunch of different stuff
</commit_message>
<xml_diff>
--- a/totalt-antal-konstaterade-covid-fall.xlsx
+++ b/totalt-antal-konstaterade-covid-fall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\DARC_Extra\Prognostisering baserad på 1177 MÅ\R-talet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F58A5BC-8C35-4779-997E-5F86931F4ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A46E56-BA59-4A87-8CBA-8678B23532FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Underlag" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="362">
   <si>
     <t>Nya konstaterade personer</t>
   </si>
@@ -1116,6 +1116,9 @@
   </si>
   <si>
     <t>22 februari 2021</t>
+  </si>
+  <si>
+    <t>23 februari 2021</t>
   </si>
 </sst>
 </file>
@@ -1449,11 +1452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C359"/>
+  <dimension ref="A1:C360"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A358" sqref="A358:A359"/>
+      <pane ySplit="1" topLeftCell="A336" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A359" sqref="A359:A360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5412,6 +5415,17 @@
         <v>263</v>
       </c>
     </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A360" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="B360" s="1">
+        <v>108840</v>
+      </c>
+      <c r="C360" s="1">
+        <v>449</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>